<commit_message>
Adding checkbox classifier + updating example xlsx + cleanup
</commit_message>
<xml_diff>
--- a/scanExample.xlsx
+++ b/scanExample.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="64">
   <si>
     <t>type</t>
   </si>
@@ -96,39 +96,21 @@
     <t>sweep</t>
   </si>
   <si>
-    <t>bathroom</t>
-  </si>
-  <si>
     <t>Name:</t>
   </si>
   <si>
     <t>bub_num 2</t>
   </si>
   <si>
-    <t>bub_word 10</t>
-  </si>
-  <si>
     <t>roomNum</t>
   </si>
   <si>
     <t>Room Number:</t>
   </si>
   <si>
-    <t>Wash dishes</t>
-  </si>
-  <si>
-    <t>Sweep patio</t>
-  </si>
-  <si>
     <t>cook</t>
   </si>
   <si>
-    <t>Cook dinner</t>
-  </si>
-  <si>
-    <t>Clean bathroom&lt;br /&gt;</t>
-  </si>
-  <si>
     <t>roomba</t>
   </si>
   <si>
@@ -150,7 +132,82 @@
     <t>Program roomba&lt;br /&gt;</t>
   </si>
   <si>
-    <t>Please turn in this chore signup form&lt;br /&gt;when you arrive at the lodge.</t>
+    <t>qrcode</t>
+  </si>
+  <si>
+    <t>bub_word 14</t>
+  </si>
+  <si>
+    <t>rows</t>
+  </si>
+  <si>
+    <t>font</t>
+  </si>
+  <si>
+    <t>13px times;</t>
+  </si>
+  <si>
+    <t>Cook dinner&lt;br /&gt;</t>
+  </si>
+  <si>
+    <t>Sweep patio&lt;br /&gt;</t>
+  </si>
+  <si>
+    <t>Wash dishes&lt;br /&gt;</t>
+  </si>
+  <si>
+    <t>No&lt;br /&gt;</t>
+  </si>
+  <si>
+    <t>Yes&lt;br /&gt;</t>
+  </si>
+  <si>
+    <t>mon_chores</t>
+  </si>
+  <si>
+    <t>tues_chores</t>
+  </si>
+  <si>
+    <t>wed_chores</t>
+  </si>
+  <si>
+    <t>thurs_chores</t>
+  </si>
+  <si>
+    <t>fri_chores</t>
+  </si>
+  <si>
+    <t>sat_chores</t>
+  </si>
+  <si>
+    <t>sun_chores</t>
+  </si>
+  <si>
+    <t>Please turn in this chore signup form when you arrive at the lodge.</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>constraint</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>integer</t>
+  </si>
+  <si>
+    <t>stay</t>
+  </si>
+  <si>
+    <t>Length of Stay (days):</t>
+  </si>
+  <si>
+    <t>count-selected(.) = 2</t>
+  </si>
+  <si>
+    <t>qrcode This text is encoded in the QR code.</t>
   </si>
 </sst>
 </file>
@@ -490,21 +547,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C43"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26" customWidth="1"/>
+    <col min="1" max="1" width="22.28515625" customWidth="1"/>
     <col min="2" max="2" width="32.28515625" customWidth="1"/>
     <col min="3" max="3" width="48.85546875" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -514,235 +573,238 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    </row>
+    <row r="11" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14"/>
+    </row>
+    <row r="15" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15"/>
+    </row>
+    <row r="16" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>38</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10"/>
-    </row>
-    <row r="11" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11"/>
-    </row>
-    <row r="12" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>10</v>
+        <v>56</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="C19" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>18</v>
       </c>
       <c r="B23" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="C23" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>13</v>
+        <v>56</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>18</v>
       </c>
       <c r="B27" t="s">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="C27" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>18</v>
       </c>
       <c r="B31" t="s">
-        <v>20</v>
+        <v>51</v>
       </c>
       <c r="C31" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>3</v>
       </c>
@@ -754,13 +816,10 @@
     </row>
     <row r="34" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>15</v>
+        <v>56</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -768,7 +827,7 @@
         <v>18</v>
       </c>
       <c r="B35" t="s">
-        <v>20</v>
+        <v>52</v>
       </c>
       <c r="C35" t="s">
         <v>19</v>
@@ -786,13 +845,10 @@
     </row>
     <row r="38" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -800,7 +856,7 @@
         <v>18</v>
       </c>
       <c r="B39" t="s">
-        <v>20</v>
+        <v>53</v>
       </c>
       <c r="C39" t="s">
         <v>19</v>
@@ -811,20 +867,49 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>3</v>
+    <row r="41" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="B43" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="C43" t="s">
-        <v>40</v>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>32</v>
+      </c>
+      <c r="B46" t="s">
+        <v>33</v>
+      </c>
+      <c r="C46" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -835,10 +920,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -866,7 +951,7 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -877,7 +962,7 @@
         <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -888,7 +973,7 @@
         <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -899,7 +984,7 @@
         <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -907,10 +992,10 @@
         <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -918,21 +1003,10 @@
         <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" t="s">
         <v>37</v>
-      </c>
-      <c r="C8" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -942,15 +1016,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -969,6 +1044,14 @@
         <v>22</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" t="s">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>